<commit_message>
Repair template import & remove useless ControllerFxCorrection
</commit_message>
<xml_diff>
--- a/fr.istic.tools.scanexam/torchon_pfo.xlsx
+++ b/fr.istic.tools.scanexam/torchon_pfo.xlsx
@@ -111,7 +111,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="3">
@@ -119,7 +119,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="4">
@@ -127,7 +127,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="5">
@@ -135,7 +135,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="6">
@@ -143,7 +143,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="7">
@@ -151,7 +151,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="8">
@@ -167,7 +167,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="10">

</xml_diff>